<commit_message>
feat(log):add log-file + csv
need implement for excel and pdf
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -484,7 +484,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.388s</t>
+          <t>0.324s</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.119s</t>
+          <t>0.311s</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.305s</t>
+          <t>0.321s</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.493s</t>
+          <t>0.311s</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.367s</t>
+          <t>0.322s</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.236s</t>
+          <t>0.232s</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -652,7 +652,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.235s</t>
+          <t>0.240s</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.234s</t>
+          <t>0.231s</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -708,7 +708,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.249s</t>
+          <t>0.234s</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.018s</t>
+          <t>0.240s</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.245s</t>
+          <t>0.456s</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -792,7 +792,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.230s</t>
+          <t>0.457s</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -820,7 +820,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.028s</t>
+          <t>0.454s</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.227s</t>
+          <t>0.229s</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.243s</t>
+          <t>0.229s</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -904,7 +904,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.020s</t>
+          <t>0.228s</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">

</xml_diff>

<commit_message>
feat(external): add external tool support
use the --external-tool and quotes to specify the tool

use the {url} place holder for the external tool for each dir

use --tooloutput-csv/excel/pdf for specifying the output file format
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Errors" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,38 +438,221 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>URL</t>
+          <t>Metric</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Size</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Server</t>
+          <t>Value</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Target URL</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://ksurajsingh.github.io</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Total Checked</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Found Items</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Success Rate</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5.7%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>19.89 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Requests/sec</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>8.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Most common status code</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>301 (8 times)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Fastest response time</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0.230s</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Slowest response time</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0.382s</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Average response time</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0.279s</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Smallest content size</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>162 bytes</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Largest content size</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10117 bytes</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Average content size</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1581 bytes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Size</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Server</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>https://ksurajsingh.github.io/media</t>
         </is>
       </c>
@@ -479,12 +664,14 @@
           <t>DIR</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>162</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>162.0 B</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.324s</t>
+          <t>0.382s</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -496,23 +683,25 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/index</t>
+          <t>https://ksurajsingh.github.io/futurediary</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>200</v>
+        <v>301</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>DIR</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>2214</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>162.0 B</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.311s</t>
+          <t>0.376s</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -524,7 +713,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/tmp</t>
+          <t>https://ksurajsingh.github.io/media/index</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -535,12 +724,14 @@
           <t>DIR</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>162</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>162.0 B</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.321s</t>
+          <t>0.250s</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -552,7 +743,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/docs</t>
+          <t>https://ksurajsingh.github.io/media/gifs</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -563,12 +754,14 @@
           <t>DIR</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>162</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>162.0 B</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.311s</t>
+          <t>0.308s</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -580,7 +773,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/futurediary</t>
+          <t>https://ksurajsingh.github.io/futurediary/futurediarymedia</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -591,12 +784,14 @@
           <t>DIR</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>162</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>162.0 B</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.322s</t>
+          <t>0.248s</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -608,7 +803,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/media/index</t>
+          <t>https://ksurajsingh.github.io/futurediary/trash</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -619,12 +814,14 @@
           <t>DIR</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>162</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>162.0 B</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.232s</t>
+          <t>0.234s</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -636,23 +833,25 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/media/gifs</t>
+          <t>https://ksurajsingh.github.io/futurediary/futurediary</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>301</v>
+        <v>200</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>DIR</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>162</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>9.9 KB</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.240s</t>
+          <t>0.230s</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -664,7 +863,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/media/vids</t>
+          <t>https://ksurajsingh.github.io/media/index/gifs</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -675,12 +874,14 @@
           <t>DIR</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>162</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>162.0 B</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.231s</t>
+          <t>0.230s</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -692,7 +893,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/media/pics</t>
+          <t>https://ksurajsingh.github.io/media/index/pics</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -703,12 +904,14 @@
           <t>DIR</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>162</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>162.0 B</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.234s</t>
+          <t>0.243s</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -720,7 +923,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/tmp/tmp</t>
+          <t>https://ksurajsingh.github.io/futurediary/trash/trash</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -731,185 +934,276 @@
           <t>DIR</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>3400</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>4.3 KB</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.240s</t>
+          <t>0.288s</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>GitHub.com</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>[ERROR] Error during scan:(str[Errno 13] Permission denied: '/root/myfile.xlsx')</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Exception: [Errno 13] Permission denied: '/root/myfile.xlsx'</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>[ERROR] Error during scan:(strdivision by zero)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Exception: division by zero</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>[ERROR] Error during scan:(strdivision by zero)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Exception: division by zero</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>[ERROR] Error during scan:(strdivision by zero)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Exception: division by zero</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>[ERROR] Error during scan:(str[Errno 13] Permission denied: '/root/report.xlsx')</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Exception: [Errno 13] Permission denied: '/root/report.xlsx'</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/futurediary/futurediarymedia</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>301</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>DIR</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>162</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>0.456s</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>GitHub.com</t>
+          <t>[ERROR] Error during scan:(str[Errno 13] Permission denied: '/root/report.xlsx')</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/futurediary/trash</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>301</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>DIR</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>162</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>0.457s</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>GitHub.com</t>
+          <t>Exception: [Errno 13] Permission denied: '/root/report.xlsx'</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/futurediary/futurediary</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>200</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>DIR</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>10117</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>0.454s</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>GitHub.com</t>
+          <t>[ERROR] Error during scan:(str[Errno 13] Permission denied: '/root/report.csv')</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/media/index/gifs</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>301</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>DIR</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>162</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>0.229s</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>GitHub.com</t>
+          <t>Exception: [Errno 13] Permission denied: '/root/report.csv'</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/media/index/pics</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>301</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>DIR</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>162</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>0.229s</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>GitHub.com</t>
+          <t>[ERROR] Error during scan:(strDirectoryEnumerator.scan_target() got an unexpected keyword argument 'custom_wordlist')</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://ksurajsingh.github.io/futurediary/trash/trash</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>200</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>DIR</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>4400</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>0.228s</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>GitHub.com</t>
+          <t>Exception: DirectoryEnumerator.scan_target() got an unexpected keyword argument 'custom_wordlist'</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>[ERROR] Error during scan:(strDirectoryEnumerator.scan_target() got an unexpected keyword argument 'recursive')</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Exception: DirectoryEnumerator.scan_target() got an unexpected keyword argument 'recursive'</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>[ERROR] Error running per-dir command: Command 'nuclei -u https://ksurajsingh.github.io/media' timed out after 120 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>KeyboardInterrupt: Scan interrupted by user.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>KeyboardInterrupt: Scan interrupted by user.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>[ERROR] Error running per-dir command: Command 'nuclei -u https://ksurajsingh.github.io/media' timed out after 120 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>[ERROR] Error running per-dir command: Command 'nuclei -u https://ksurajsingh.github.io/futurediary' timed out after 120 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>KeyboardInterrupt: Scan interrupted by user.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>[ERROR] Error during scan:(strname 'status_to_pdf_color' is not defined)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Exception: name 'status_to_pdf_color' is not defined</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>[ERROR] Error during scan:(strname 'status_to_pdf_color' is not defined)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Exception: name 'status_to_pdf_color' is not defined</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>[ERROR] Error during scan:(strname 'type_to_pdf_color' is not defined)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Exception: name 'type_to_pdf_color' is not defined</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>[ERROR] Error running per-dir command: Command 'nuclei -u https://ksurajsingh.github.io/media' timed out after 120 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>[ERROR] Error running per-dir command: Command 'nuclei -u https://ksurajsingh.github.io/index' timed out after 120 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>KeyboardInterrupt: Scan interrupted by user.</t>
         </is>
       </c>
     </row>

</xml_diff>